<commit_message>
Add environment file for conda
</commit_message>
<xml_diff>
--- a/datasets/excel/glink_distribution.xlsx
+++ b/datasets/excel/glink_distribution.xlsx
@@ -453,14 +453,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>glink_original</t>
+          <t>glink_ce_blanked</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>